<commit_message>
fixed theoretical data again
</commit_message>
<xml_diff>
--- a/DATA.new.xlsx
+++ b/DATA.new.xlsx
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1192,7 +1192,7 @@
         <v>33.216830283527621</v>
       </c>
       <c r="Z2" s="2">
-        <f>1/(1+(0.000000000000107506/(9.109E-31*POWER(300000000,2)))*(1-COS(RADIANS(A2))))</f>
+        <f t="shared" ref="Z2:Z15" si="1">1/(1+(1.0606413726E-13/(9.109E-31*POWER(300000000,2)))*(1-COS(RADIANS(A2))))</f>
         <v>1</v>
       </c>
     </row>
@@ -1233,15 +1233,15 @@
         <v>315.34605191871367</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L15" si="1">J3/B3</f>
+        <f t="shared" ref="L3:L15" si="2">J3/B3</f>
         <v>9.5510751771421951</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M15" si="2">K3/B3</f>
+        <f t="shared" ref="M3:M15" si="3">K3/B3</f>
         <v>1.5767302595935684</v>
       </c>
       <c r="N3" s="11">
-        <f t="shared" ref="N3:N15" si="3">(E3+61.6)/11540.4</f>
+        <f t="shared" ref="N3:N15" si="4">(E3+61.6)/11540.4</f>
         <v>0.64402966968216013</v>
       </c>
       <c r="O3" s="11">
@@ -1260,7 +1260,7 @@
         <v>0.40589999999999998</v>
       </c>
       <c r="S3" s="4">
-        <f t="shared" ref="S3:S15" si="4">R3*0.05</f>
+        <f t="shared" ref="S3:S15" si="5">R3*0.05</f>
         <v>2.0295000000000001E-2</v>
       </c>
       <c r="T3" s="2">
@@ -1276,20 +1276,20 @@
         <v>2.460449021491582E-26</v>
       </c>
       <c r="W3" s="11">
-        <f t="shared" ref="W3:W15" si="5">V3*1E+24</f>
+        <f t="shared" ref="W3:W15" si="6">V3*1E+24</f>
         <v>2.4604490214915817E-2</v>
       </c>
       <c r="X3" s="11">
-        <f t="shared" ref="X3:X15" si="6">0.5*POWER(1/137,2)*POWER(0.0000000000386,2)*POWER(Z3,2)*(Z3+1/Z3-1+POWER(COS(RADIANS(A3)),2))*1E+24</f>
-        <v>7.517740944578237E-2</v>
+        <f t="shared" ref="X3:X15" si="7">0.5*POWER(1/137,2)*POWER(0.0000000000386,2)*POWER(Z3,2)*(Z3+1/Z3-1+POWER(COS(RADIANS(A3)),2))*1E+24</f>
+        <v>7.5216422611297101E-2</v>
       </c>
       <c r="Y3" s="13">
-        <f t="shared" ref="Y3:Y15" si="7">POWER((U3-X3)/W3,2)</f>
-        <v>2.0350355107432589</v>
+        <f t="shared" ref="Y3:Y15" si="8">POWER((U3-X3)/W3,2)</f>
+        <v>2.0305141268420011</v>
       </c>
       <c r="Z3" s="2">
-        <f t="shared" ref="Z3:Z15" si="8">1/(1+(0.000000000000107506/(9.109E-31*POWER(300000000,2)))*(1-COS(RADIANS(A3))))</f>
-        <v>0.98046675591573962</v>
+        <f t="shared" si="1"/>
+        <v>0.98072368440096847</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -1329,15 +1329,15 @@
         <v>507.76705531487812</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.1193584856344803</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.84627842552479682</v>
       </c>
       <c r="N4" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.61049010432913942</v>
       </c>
       <c r="O4" s="11">
@@ -1356,7 +1356,7 @@
         <v>0.43380000000000002</v>
       </c>
       <c r="S4" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1690000000000001E-2</v>
       </c>
       <c r="T4" s="2">
@@ -1372,20 +1372,20 @@
         <v>1.7385341299552656E-26</v>
       </c>
       <c r="W4" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7385341299552656E-2</v>
       </c>
       <c r="X4" s="11">
-        <f t="shared" si="6"/>
-        <v>6.4384737830657068E-2</v>
+        <f t="shared" si="7"/>
+        <v>6.450641222663403E-2</v>
       </c>
       <c r="Y4" s="13">
-        <f t="shared" si="7"/>
-        <v>3.8552175489379357</v>
+        <f t="shared" si="8"/>
+        <v>3.8277831329508429</v>
       </c>
       <c r="Z4" s="2">
-        <f>1/(1+(0.000000000000107506/(9.109E-31*POWER(300000000,2)))*(1-COS(RADIANS(A4))))</f>
-        <v>0.92671170849175111</v>
+        <f t="shared" si="1"/>
+        <v>0.92762350422949846</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -1429,11 +1429,11 @@
         <v>8.1331333370195207</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.83364592047211683</v>
       </c>
       <c r="N5" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.56365637239610422</v>
       </c>
       <c r="O5" s="11">
@@ -1452,7 +1452,7 @@
         <v>0.44819999999999999</v>
       </c>
       <c r="S5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.2409999999999999E-2</v>
       </c>
       <c r="T5" s="2">
@@ -1468,20 +1468,20 @@
         <v>1.5456754410878626E-26</v>
       </c>
       <c r="W5" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5456754410878626E-2</v>
       </c>
       <c r="X5" s="11">
-        <f t="shared" si="6"/>
-        <v>5.1006364300052669E-2</v>
+        <f t="shared" si="7"/>
+        <v>5.1192746571714881E-2</v>
       </c>
       <c r="Y5" s="13">
-        <f t="shared" si="7"/>
-        <v>4.8489751573456603</v>
+        <f t="shared" si="8"/>
+        <v>4.7960148439948123</v>
       </c>
       <c r="Z5" s="2">
-        <f t="shared" si="8"/>
-        <v>0.85056584037900029</v>
+        <f t="shared" si="1"/>
+        <v>0.85227396803730171</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -1521,7 +1521,7 @@
         <v>879.10496572965008</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.8201823782477788</v>
       </c>
       <c r="M6" s="2">
@@ -1529,7 +1529,7 @@
         <v>0.67623458902280775</v>
       </c>
       <c r="N6" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44842466465633773</v>
       </c>
       <c r="O6" s="11">
@@ -1548,7 +1548,7 @@
         <v>0.5544</v>
       </c>
       <c r="S6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7720000000000002E-2</v>
       </c>
       <c r="T6" s="2">
@@ -1564,20 +1564,20 @@
         <v>9.3385906482735598E-27</v>
       </c>
       <c r="W6" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.3385906482735589E-3</v>
       </c>
       <c r="X6" s="11">
-        <f t="shared" si="6"/>
-        <v>3.855616972340576E-2</v>
+        <f t="shared" si="7"/>
+        <v>3.8760419859286056E-2</v>
       </c>
       <c r="Y6" s="13">
-        <f t="shared" si="7"/>
-        <v>1.2990571357382013</v>
+        <f t="shared" si="8"/>
+        <v>1.249678619026199</v>
       </c>
       <c r="Z6" s="2">
-        <f>1/(1+(0.000000000000107506/(9.109E-31*POWER(300000000,2)))*(1-COS(RADIANS(A6))))</f>
-        <v>0.76522907153389874</v>
+        <f t="shared" si="1"/>
+        <v>0.76764618271868046</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1621,11 +1621,11 @@
         <v>4.4875678951763485</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.62710630135256873</v>
       </c>
       <c r="N7" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.40097396970642274</v>
       </c>
       <c r="O7" s="11">
@@ -1644,7 +1644,7 @@
         <v>0.60929999999999995</v>
       </c>
       <c r="S7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.0464999999999999E-2</v>
       </c>
       <c r="T7" s="2">
@@ -1660,20 +1660,20 @@
         <v>7.0785570531895322E-27</v>
       </c>
       <c r="W7" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.0785570531895319E-3</v>
       </c>
       <c r="X7" s="11">
-        <f t="shared" si="6"/>
-        <v>2.8763760580229697E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.8949160046953033E-2</v>
       </c>
       <c r="Y7" s="13">
-        <f t="shared" si="7"/>
-        <v>0.66055883269850346</v>
+        <f t="shared" si="8"/>
+        <v>0.6186703443709366</v>
       </c>
       <c r="Z7" s="2">
-        <f t="shared" si="8"/>
-        <v>0.68099878194495367</v>
+        <f t="shared" si="1"/>
+        <v>0.68392490087238444</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1713,15 +1713,15 @@
         <v>1142.0838563081095</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.1631795330806307</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.63449103128228301</v>
       </c>
       <c r="N8" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.35727271151779832</v>
       </c>
       <c r="O8" s="11">
@@ -1740,7 +1740,7 @@
         <v>0.66239999999999999</v>
       </c>
       <c r="S8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3120000000000004E-2</v>
       </c>
       <c r="T8" s="2">
@@ -1756,20 +1756,20 @@
         <v>6.3005202249277359E-27</v>
       </c>
       <c r="W8" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.3005202249277357E-3</v>
       </c>
       <c r="X8" s="11">
-        <f t="shared" si="6"/>
-        <v>2.18590607833666E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.2011629877978396E-2</v>
       </c>
       <c r="Y8" s="13">
-        <f t="shared" si="7"/>
-        <v>1.453405340120121</v>
+        <f t="shared" si="8"/>
+        <v>1.3956050753799336</v>
       </c>
       <c r="Z8" s="2">
-        <f t="shared" si="8"/>
-        <v>0.60398278986841902</v>
+        <f t="shared" si="1"/>
+        <v>0.60720788610965448</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1809,15 +1809,15 @@
         <v>1357.6411072417354</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.6487223986373549</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.6464957653532073</v>
       </c>
       <c r="N9" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.32163529860316797</v>
       </c>
       <c r="O9" s="11">
@@ -1836,7 +1836,7 @@
         <v>0.69750000000000001</v>
       </c>
       <c r="S9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.4875000000000003E-2</v>
       </c>
       <c r="T9" s="2">
@@ -1852,20 +1852,20 @@
         <v>5.692866681994198E-27</v>
       </c>
       <c r="W9" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.6928666819941976E-3</v>
       </c>
       <c r="X9" s="11">
-        <f t="shared" si="6"/>
-        <v>1.7347295999573225E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.7469689709798761E-2</v>
       </c>
       <c r="Y9" s="13">
-        <f t="shared" si="7"/>
-        <v>1.5856484672278772</v>
+        <f t="shared" si="8"/>
+        <v>1.5319652986410537</v>
       </c>
       <c r="Z9" s="2">
-        <f t="shared" si="8"/>
-        <v>0.53681371398402178</v>
+        <f t="shared" si="1"/>
+        <v>0.54016936554391659</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1905,15 +1905,15 @@
         <v>3371.6901474905908</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6218842121750261</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.46829029826258206</v>
       </c>
       <c r="N10" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.28177099580603793</v>
       </c>
       <c r="O10" s="11">
@@ -1932,7 +1932,7 @@
         <v>0.73260000000000003</v>
       </c>
       <c r="S10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6630000000000003E-2</v>
       </c>
       <c r="T10" s="2">
@@ -1948,20 +1948,20 @@
         <v>3.913019391400378E-27</v>
       </c>
       <c r="W10" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.9130193914003776E-3</v>
       </c>
       <c r="X10" s="11">
-        <f t="shared" si="6"/>
-        <v>1.4570392197332485E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.4672308838124934E-2</v>
       </c>
       <c r="Y10" s="13">
-        <f t="shared" si="7"/>
-        <v>0.31670358441978702</v>
+        <f t="shared" si="8"/>
+        <v>0.2880669748636252</v>
       </c>
       <c r="Z10" s="2">
-        <f t="shared" si="8"/>
-        <v>0.4799296685896936</v>
+        <f t="shared" si="1"/>
+        <v>0.48330076190820936</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2001,15 +2001,15 @@
         <v>3523.0050607091171</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2397041250592054</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.32620417228788123</v>
       </c>
       <c r="N11" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.27585612283802985</v>
       </c>
       <c r="O11" s="11">
@@ -2028,7 +2028,7 @@
         <v>0.76590000000000003</v>
       </c>
       <c r="S11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8295000000000003E-2</v>
       </c>
       <c r="T11" s="2">
@@ -2044,20 +2044,20 @@
         <v>2.8662378652951461E-27</v>
       </c>
       <c r="W11" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.8662378652951461E-3</v>
       </c>
       <c r="X11" s="11">
-        <f t="shared" si="6"/>
-        <v>1.2957388325761274E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.3049198576292342E-2</v>
       </c>
       <c r="Y11" s="13">
-        <f t="shared" si="7"/>
-        <v>6.7981064833511393E-2</v>
+        <f t="shared" si="8"/>
+        <v>5.2303765116596956E-2</v>
       </c>
       <c r="Z11" s="2">
-        <f t="shared" si="8"/>
-        <v>0.43264709452363481</v>
+        <f t="shared" si="1"/>
+        <v>0.4359644774363361</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -2097,15 +2097,15 @@
         <v>343.74529963574275</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.554510740825323</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.7187264981787138</v>
       </c>
       <c r="N12" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.56815621642230774</v>
       </c>
       <c r="O12" s="11">
@@ -2124,7 +2124,7 @@
         <v>0.46079999999999999</v>
       </c>
       <c r="S12" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3040000000000001E-2</v>
       </c>
       <c r="T12" s="2">
@@ -2140,20 +2140,20 @@
         <v>2.3772614603616846E-26</v>
       </c>
       <c r="W12" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.3772614603616845E-2</v>
       </c>
       <c r="X12" s="11">
-        <f t="shared" si="6"/>
-        <v>7.517740944578237E-2</v>
+        <f t="shared" si="7"/>
+        <v>7.5216422611297101E-2</v>
       </c>
       <c r="Y12" s="13">
-        <f t="shared" si="7"/>
-        <v>1.8308377746029338</v>
+        <f t="shared" si="8"/>
+        <v>1.8263993819538786</v>
       </c>
       <c r="Z12" s="2">
-        <f t="shared" si="8"/>
-        <v>0.98046675591573962</v>
+        <f t="shared" si="1"/>
+        <v>0.98072368440096847</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -2193,15 +2193,15 @@
         <v>576.79132013326102</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4975136026277891</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.96131886688876833</v>
       </c>
       <c r="N13" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.53572753110810722</v>
       </c>
       <c r="O13" s="11">
@@ -2220,7 +2220,7 @@
         <v>0.48780000000000001</v>
       </c>
       <c r="S13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4390000000000002E-2</v>
       </c>
       <c r="T13" s="2">
@@ -2236,20 +2236,20 @@
         <v>1.5344371520184826E-26</v>
       </c>
       <c r="W13" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5344371520184827E-2</v>
       </c>
       <c r="X13" s="11">
-        <f t="shared" si="6"/>
-        <v>6.4384737830657068E-2</v>
+        <f t="shared" si="7"/>
+        <v>6.450641222663403E-2</v>
       </c>
       <c r="Y13" s="13">
-        <f t="shared" si="7"/>
-        <v>1.2645283146307551</v>
+        <f t="shared" si="8"/>
+        <v>1.246757373266189</v>
       </c>
       <c r="Z13" s="2">
-        <f>1/(1+(0.000000000000107506/(9.109E-31*POWER(300000000,2)))*(1-COS(RADIANS(A13))))</f>
-        <v>0.92671170849175111</v>
+        <f t="shared" si="1"/>
+        <v>0.92762350422949846</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -2289,15 +2289,15 @@
         <v>663.06653941579521</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.7133125432608276</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.82883317426974401</v>
       </c>
       <c r="N14" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.53980711240511592</v>
       </c>
       <c r="O14" s="11">
@@ -2316,7 +2316,7 @@
         <v>0.46079999999999999</v>
       </c>
       <c r="S14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3040000000000001E-2</v>
       </c>
       <c r="T14" s="2">
@@ -2332,20 +2332,20 @@
         <v>1.3939496969267884E-26</v>
       </c>
       <c r="W14" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3939496969267884E-2</v>
       </c>
       <c r="X14" s="11">
-        <f t="shared" si="6"/>
-        <v>5.1006364300052669E-2</v>
+        <f t="shared" si="7"/>
+        <v>5.1192746571714881E-2</v>
       </c>
       <c r="Y14" s="13">
-        <f t="shared" si="7"/>
-        <v>3.8753691885529231</v>
+        <f t="shared" si="8"/>
+        <v>3.8229045542098246</v>
       </c>
       <c r="Z14" s="2">
-        <f t="shared" si="8"/>
-        <v>0.85056584037900029</v>
+        <f t="shared" si="1"/>
+        <v>0.85227396803730171</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -2385,15 +2385,15 @@
         <v>869.15658300412088</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5655897986753917</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.66858198692624682</v>
       </c>
       <c r="N15" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.49143790509861013</v>
       </c>
       <c r="O15" s="11">
@@ -2412,7 +2412,7 @@
         <v>0.504</v>
       </c>
       <c r="S15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.52E-2</v>
       </c>
       <c r="T15" s="2">
@@ -2428,20 +2428,20 @@
         <v>1.1073256759218936E-26</v>
       </c>
       <c r="W15" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1073256759218936E-2</v>
       </c>
       <c r="X15" s="11">
-        <f t="shared" si="6"/>
-        <v>3.855616972340576E-2</v>
+        <f t="shared" si="7"/>
+        <v>3.8760419859286056E-2</v>
       </c>
       <c r="Y15" s="13">
-        <f t="shared" si="7"/>
-        <v>4.1268958344488551</v>
+        <f t="shared" si="8"/>
+        <v>4.0522934694670854</v>
       </c>
       <c r="Z15" s="2">
-        <f t="shared" si="8"/>
-        <v>0.76522907153389874</v>
+        <f t="shared" si="1"/>
+        <v>0.76764618271868046</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="K20" s="4">
         <f>SUM(Y3:Y15)</f>
-        <v>27.220213754300325</v>
+        <v>26.738956960082977</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="K22">
         <f>K20/K21</f>
-        <v>2.0938625964846405</v>
+        <v>2.0568428430833059</v>
       </c>
     </row>
     <row r="23" spans="1:15">

</xml_diff>

<commit_message>
changed data, need new plots, updated efficiency table
</commit_message>
<xml_diff>
--- a/DATA.new.xlsx
+++ b/DATA.new.xlsx
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1145,19 +1145,19 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2">
         <f xml:space="preserve"> SQRT(2*3.14159)*G2*C2/(B17*T2)</f>
-        <v>466991.61160205182</v>
+        <v>442140.61674961442</v>
       </c>
       <c r="K2" s="2">
         <f>SQRT(2*3.14159*POWER(1/40.96,2)*(POWER(C2*H2/T2,2)+POWER(G2*D2/T2,2)+POWER(C2*G2*U2/POWER(T2,2),2)))</f>
-        <v>46762.286461201053</v>
+        <v>44273.827758165971</v>
       </c>
       <c r="L2" s="2">
         <f>J2/B2</f>
-        <v>7783.1935267008639</v>
+        <v>7369.0102791602403</v>
       </c>
       <c r="M2" s="2">
         <f>K2/B2</f>
-        <v>779.37144102001753</v>
+        <v>737.89712930276619</v>
       </c>
       <c r="N2" s="11">
         <f>(E2+61.6)/11540.4</f>
@@ -1184,27 +1184,27 @@
         <v>0.13083539949272774</v>
       </c>
       <c r="T2" s="4">
-        <v>0.38429999999999997</v>
+        <v>0.40589999999999998</v>
       </c>
       <c r="U2" s="4">
         <f>T2*0.05</f>
-        <v>1.9214999999999999E-2</v>
+        <v>2.0295000000000001E-2</v>
       </c>
       <c r="V2" s="2">
         <f>L2/(L2*T2*B27*B25)</f>
-        <v>9.4915827816779713E-23</v>
+        <v>8.9864874673536425E-23</v>
       </c>
       <c r="W2" s="11">
         <f>V2*1E+24</f>
-        <v>94.915827816779711</v>
+        <v>89.86487467353642</v>
       </c>
       <c r="X2" s="2">
         <f>SQRT(POWER(M2/(L2*T2*B27*B25),2)+POWER(L2*M2/(POWER(L2,2)*T2*B27*B25),2)+POWER(L2*C27/(L2*T2*POWER(B27,2)*B25),2)+POWER(L2*C25/(L2*T2*B27*POWER(B25,2)),2))</f>
-        <v>1.6454934815612501E-23</v>
+        <v>1.5579284182409179E-23</v>
       </c>
       <c r="Y2" s="11">
         <f>X2*1E+24</f>
-        <v>16.4549348156125</v>
+        <v>15.579284182409179</v>
       </c>
       <c r="Z2" s="11">
         <f>0.5*POWER(1/137,2)*POWER(0.0000000000386,2)*POWER(AB2,2)*(AB2+1/AB2-1+POWER(COS(RADIANS(A2)),2))*1E+24</f>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="AA2" s="13">
         <f>POWER((W2-Z2)/Y2,2)</f>
-        <v>33.216830283527621</v>
+        <v>33.213704783202196</v>
       </c>
       <c r="AB2" s="2">
         <f t="shared" ref="AB2:AB15" si="1">1/(1+(1.0606413726E-13/(9.109E-31*POWER(300000000,2)))*(1-COS(RADIANS(A2))))</f>
@@ -1296,19 +1296,19 @@
       </c>
       <c r="V3" s="2">
         <f>L3/(L2*T3*B27*B25)</f>
-        <v>1.1027686396938746E-25</v>
+        <v>1.1647509519951697E-25</v>
       </c>
       <c r="W3" s="11">
         <f>V3*1E+24</f>
-        <v>0.11027686396938746</v>
+        <v>0.11647509519951697</v>
       </c>
       <c r="X3" s="2">
         <f>SQRT(POWER(M3/(L2*T3*B27*B25),2)+POWER(L3*M2/(POWER(L2,2)*T3*B27*B25),2)+POWER(L3*C27/(L2*T3*POWER(B27,2)*B25),2)+POWER(L3*C25/(L2*T3*B27*POWER(B25,2)),2)+POWER(L3*U3/(L2*POWER(T3,2)*B27*B25),2))</f>
-        <v>2.460449021491582E-26</v>
+        <v>2.5987412381562144E-26</v>
       </c>
       <c r="Y3" s="11">
         <f t="shared" ref="Y3:Y15" si="8">X3*1E+24</f>
-        <v>2.4604490214915817E-2</v>
+        <v>2.5987412381562144E-2</v>
       </c>
       <c r="Z3" s="11">
         <f t="shared" ref="Z3:Z15" si="9">0.5*POWER(1/137,2)*POWER(0.0000000000386,2)*POWER(AB3,2)*(AB3+1/AB3-1+POWER(COS(RADIANS(A3)),2))*1E+24</f>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="AA3" s="13">
         <f t="shared" ref="AA3:AA15" si="10">POWER((W3-Z3)/Y3,2)</f>
-        <v>2.0305141268420011</v>
+        <v>2.5206028705470716</v>
       </c>
       <c r="AB3" s="2">
         <f t="shared" si="1"/>
@@ -1392,27 +1392,27 @@
         <v>1.920757324366824E-2</v>
       </c>
       <c r="T4" s="4">
-        <v>0.43380000000000002</v>
+        <v>0.42120000000000002</v>
       </c>
       <c r="U4" s="4">
         <f t="shared" si="7"/>
-        <v>2.1690000000000001E-2</v>
+        <v>2.1060000000000002E-2</v>
       </c>
       <c r="V4" s="2">
         <f>L4/(L2*T4*B27*B25)</f>
-        <v>9.8520347671986592E-26</v>
+        <v>1.0717063100558357E-25</v>
       </c>
       <c r="W4" s="11">
         <f>V4*1E+24</f>
-        <v>9.8520347671986586E-2</v>
+        <v>0.10717063100558356</v>
       </c>
       <c r="X4" s="2">
         <f>SQRT(POWER(M4/(L2*T4*B27*B25),2)+POWER(L4*M2/(POWER(L2,2)*T4*B27*B25),2)+POWER(L4*C27/(L2*T4*POWER(B27,2)*B25),2)+POWER(L4*C25/(L2*T4*B27*POWER(B25,2)),2)+POWER(L4*U4/(L2*POWER(T4,2)*B27*B25),2))</f>
-        <v>1.7385341299552656E-26</v>
+        <v>1.8911808995272905E-26</v>
       </c>
       <c r="Y4" s="11">
         <f t="shared" si="8"/>
-        <v>1.7385341299552656E-2</v>
+        <v>1.8911808995272904E-2</v>
       </c>
       <c r="Z4" s="11">
         <f t="shared" si="9"/>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="AA4" s="13">
         <f t="shared" si="10"/>
-        <v>3.8277831329508429</v>
+        <v>5.0893398132282481</v>
       </c>
       <c r="AB4" s="2">
         <f t="shared" si="1"/>
@@ -1496,27 +1496,27 @@
         <v>4.5046095369574208E-4</v>
       </c>
       <c r="T5" s="4">
-        <v>0.44819999999999999</v>
+        <v>0.46079999999999999</v>
       </c>
       <c r="U5" s="4">
         <f t="shared" si="7"/>
-        <v>2.2409999999999999E-2</v>
+        <v>2.3040000000000001E-2</v>
       </c>
       <c r="V5" s="2">
         <f>L5/(L2*T5*B27*B25)</f>
-        <v>8.5042738219826426E-26</v>
+        <v>8.7366569629576684E-26</v>
       </c>
       <c r="W5" s="11">
         <f t="shared" ref="W5:W15" si="14">V5*1E+24</f>
-        <v>8.5042738219826428E-2</v>
+        <v>8.7366569629576687E-2</v>
       </c>
       <c r="X5" s="2">
         <f>SQRT(POWER(M5/(L2*T5*B27*B25),2)+POWER(L5*M2/(POWER(L2,2)*T5*B27*B25),2)+POWER(L5*C27/(L2*T5*POWER(B27,2)*B25),2)+POWER(L5*C25/(L2*T5*B27*POWER(B25,2)),2)+POWER(L5*U5/(L2*POWER(T5,2)*B27*B25),2))</f>
-        <v>1.5456754410878626E-26</v>
+        <v>1.587911723861295E-26</v>
       </c>
       <c r="Y5" s="11">
         <f t="shared" si="8"/>
-        <v>1.5456754410878626E-2</v>
+        <v>1.587911723861295E-2</v>
       </c>
       <c r="Z5" s="11">
         <f t="shared" si="9"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="AA5" s="13">
         <f t="shared" si="10"/>
-        <v>4.7960148439948123</v>
+        <v>5.1896265820465155</v>
       </c>
       <c r="AB5" s="2">
         <f t="shared" si="1"/>
@@ -1600,27 +1600,27 @@
         <v>5.1892745478269999</v>
       </c>
       <c r="T6" s="4">
-        <v>0.5544</v>
+        <v>0.504</v>
       </c>
       <c r="U6" s="4">
         <f t="shared" si="7"/>
-        <v>2.7720000000000002E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="V6" s="2">
         <f>L6/(L2*T6*B27*B25)</f>
-        <v>4.9199939327068512E-26</v>
+        <v>5.7161803044868141E-26</v>
       </c>
       <c r="W6" s="11">
         <f t="shared" si="14"/>
-        <v>4.9199939327068509E-2</v>
+        <v>5.7161803044868141E-2</v>
       </c>
       <c r="X6" s="2">
         <f>SQRT(POWER(M6/(L2*T6*B27*B25),2)+POWER(L6*M2/(POWER(L2,2)*T6*B27*B25),2)+POWER(L6*C27/(L2*T6*POWER(B27,2)*B25),2)+POWER(L6*C25/(L2*T6*B27*POWER(B25,2)),2)+POWER(L6*U6/(L2*POWER(T6,2)*B27*B25),2))</f>
-        <v>9.3385906482735598E-27</v>
+        <v>1.0849823935851321E-26</v>
       </c>
       <c r="Y6" s="11">
         <f t="shared" si="8"/>
-        <v>9.3385906482735589E-3</v>
+        <v>1.0849823935851322E-2</v>
       </c>
       <c r="Z6" s="11">
         <f t="shared" si="9"/>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="AA6" s="13">
         <f t="shared" si="10"/>
-        <v>1.249678619026199</v>
+        <v>2.8764415703301003</v>
       </c>
       <c r="AB6" s="2">
         <f t="shared" si="1"/>
@@ -1704,27 +1704,27 @@
         <v>3.8941994367224462</v>
       </c>
       <c r="T7" s="4">
-        <v>0.60929999999999995</v>
+        <v>0.5544</v>
       </c>
       <c r="U7" s="4">
         <f t="shared" si="7"/>
-        <v>3.0464999999999999E-2</v>
+        <v>2.7720000000000002E-2</v>
       </c>
       <c r="V7" s="2">
         <f>L7/(L2*T7*B27*B25)</f>
-        <v>3.4516841583037877E-26</v>
+        <v>4.0067078112260882E-26</v>
       </c>
       <c r="W7" s="11">
         <f t="shared" si="14"/>
-        <v>3.4516841583037874E-2</v>
+        <v>4.006707811226088E-2</v>
       </c>
       <c r="X7" s="2">
         <f>SQRT(POWER(M7/(L2*T7*B27*B25),2)+POWER(L7*M2/(POWER(L2,2)*T7*B27*B25),2)+POWER(L7*C27/(L2*T7*POWER(B27,2)*B25),2)+POWER(L7*C25/(L2*T7*B27*POWER(B25,2)),2)+POWER(L7*U7/(L2*POWER(T7,2)*B27*B25),2))</f>
-        <v>7.0785570531895322E-27</v>
+        <v>8.216774344487364E-27</v>
       </c>
       <c r="Y7" s="11">
         <f t="shared" si="8"/>
-        <v>7.0785570531895319E-3</v>
+        <v>8.2167743444873636E-3</v>
       </c>
       <c r="Z7" s="11">
         <f t="shared" si="9"/>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="AA7" s="13">
         <f t="shared" si="10"/>
-        <v>0.6186703443709366</v>
+        <v>1.830813970931277</v>
       </c>
       <c r="AB7" s="2">
         <f t="shared" si="1"/>
@@ -1808,27 +1808,27 @@
         <v>2.8673726518399776</v>
       </c>
       <c r="T8" s="4">
-        <v>0.66239999999999999</v>
+        <v>0.60929999999999995</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" si="7"/>
-        <v>3.3120000000000004E-2</v>
+        <v>3.0464999999999999E-2</v>
       </c>
       <c r="V8" s="2">
         <f>L8/(L2*T8*B27*B25)</f>
-        <v>2.9454795453138688E-26</v>
+        <v>3.3821574668284608E-26</v>
       </c>
       <c r="W8" s="11">
         <f t="shared" si="14"/>
-        <v>2.9454795453138689E-2</v>
+        <v>3.3821574668284608E-2</v>
       </c>
       <c r="X8" s="2">
         <f>SQRT(POWER(M8/(L2*T8*B27*B25),2)+POWER(L8*M2/(POWER(L2,2)*T8*B27*B25),2)+POWER(L8*C27/(L2*T8*POWER(B27,2)*B25),2)+POWER(L8*C25/(L2*T8*B27*POWER(B25,2)),2)+POWER(L8*U8/(L2*POWER(T8,2)*B27*B25),2))</f>
-        <v>6.3005202249277359E-27</v>
+        <v>7.2345949770879719E-27</v>
       </c>
       <c r="Y8" s="11">
         <f t="shared" si="8"/>
-        <v>6.3005202249277357E-3</v>
+        <v>7.2345949770879717E-3</v>
       </c>
       <c r="Z8" s="11">
         <f t="shared" si="9"/>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="AA8" s="13">
         <f t="shared" si="10"/>
-        <v>1.3956050753799336</v>
+        <v>2.6648163830246312</v>
       </c>
       <c r="AB8" s="2">
         <f t="shared" si="1"/>
@@ -1912,27 +1912,27 @@
         <v>1.8317086972870662</v>
       </c>
       <c r="T9" s="4">
-        <v>0.69750000000000001</v>
+        <v>0.66239999999999999</v>
       </c>
       <c r="U9" s="4">
         <f t="shared" si="7"/>
-        <v>3.4875000000000003E-2</v>
+        <v>3.3120000000000004E-2</v>
       </c>
       <c r="V9" s="2">
         <f>L9/(L2*T9*B27*B25)</f>
-        <v>2.4515898006132092E-26</v>
+        <v>2.7265932856230659E-26</v>
       </c>
       <c r="W9" s="11">
         <f t="shared" si="14"/>
-        <v>2.4515898006132093E-2</v>
+        <v>2.7265932856230659E-2</v>
       </c>
       <c r="X9" s="2">
         <f>SQRT(POWER(M9/(L2*T9*B27*B25),2)+POWER(L9*M2/(POWER(L2,2)*T9*B27*B25),2)+POWER(L9*C27/(L2*T9*POWER(B27,2)*B25),2)+POWER(L9*C25/(L2*T9*B27*POWER(B25,2)),2)+POWER(L9*U9/(L2*POWER(T9,2)*B27*B25),2))</f>
-        <v>5.692866681994198E-27</v>
+        <v>6.3314556404134706E-27</v>
       </c>
       <c r="Y9" s="11">
         <f t="shared" si="8"/>
-        <v>5.6928666819941976E-3</v>
+        <v>6.3314556404134702E-3</v>
       </c>
       <c r="Z9" s="11">
         <f t="shared" si="9"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="AA9" s="13">
         <f t="shared" si="10"/>
-        <v>1.5319652986410537</v>
+        <v>2.3939329090650809</v>
       </c>
       <c r="AB9" s="2">
         <f t="shared" si="1"/>
@@ -2016,27 +2016,27 @@
         <v>2.1580936427924606</v>
       </c>
       <c r="T10" s="4">
-        <v>0.73260000000000003</v>
+        <v>0.69750000000000001</v>
       </c>
       <c r="U10" s="4">
         <f t="shared" si="7"/>
-        <v>3.6630000000000003E-2</v>
+        <v>3.4875000000000003E-2</v>
       </c>
       <c r="V10" s="2">
         <f>L10/(L2*T10*B27*B25)</f>
-        <v>1.6772499562455111E-26</v>
+        <v>1.8606691559631778E-26</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="14"/>
-        <v>1.677249956245511E-2</v>
+        <v>1.8606691559631777E-2</v>
       </c>
       <c r="X10" s="2">
         <f>SQRT(POWER(M10/(L2*T10*B27*B25),2)+POWER(L10*M2/(POWER(L2,2)*T10*B27*B25),2)+POWER(L10*C27/(L2*T10*POWER(B27,2)*B25),2)+POWER(L10*C25/(L2*T10*B27*POWER(B25,2)),2)+POWER(L10*U10/(L2*POWER(T10,2)*B27*B25),2))</f>
-        <v>3.913019391400378E-27</v>
+        <v>4.3409358641823936E-27</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="8"/>
-        <v>3.9130193914003776E-3</v>
+        <v>4.3409358641823938E-3</v>
       </c>
       <c r="Z10" s="11">
         <f t="shared" si="9"/>
@@ -2044,7 +2044,7 @@
       </c>
       <c r="AA10" s="13">
         <f t="shared" si="10"/>
-        <v>0.2880669748636252</v>
+        <v>0.82146009217383864</v>
       </c>
       <c r="AB10" s="2">
         <f t="shared" si="1"/>
@@ -2120,27 +2120,27 @@
         <v>0.24302702065583023</v>
       </c>
       <c r="T11" s="4">
-        <v>0.76590000000000003</v>
+        <v>0.73260000000000003</v>
       </c>
       <c r="U11" s="4">
         <f t="shared" si="7"/>
-        <v>3.8295000000000003E-2</v>
+        <v>3.6630000000000003E-2</v>
       </c>
       <c r="V11" s="2">
         <f>L11/(L2*T11*B27*B25)</f>
-        <v>1.3704707646793601E-26</v>
+        <v>1.5132950012794341E-26</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="14"/>
-        <v>1.37047076467936E-2</v>
+        <v>1.5132950012794341E-2</v>
       </c>
       <c r="X11" s="2">
         <f>SQRT(POWER(M11/(L2*T11*B27*B25),2)+POWER(L11*M2/(POWER(L2,2)*T11*B27*B25),2)+POWER(L11*C27/(L2*T11*POWER(B27,2)*B25),2)+POWER(L11*C25/(L2*T11*B27*POWER(B25,2)),2)+POWER(L11*U11/(L2*POWER(T11,2)*B27*B25),2))</f>
-        <v>2.8662378652951461E-27</v>
+        <v>3.1649441533645471E-27</v>
       </c>
       <c r="Y11" s="11">
         <f t="shared" si="8"/>
-        <v>2.8662378652951461E-3</v>
+        <v>3.164944153364547E-3</v>
       </c>
       <c r="Z11" s="11">
         <f t="shared" si="9"/>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="AA11" s="13">
         <f t="shared" si="10"/>
-        <v>5.2303765116596956E-2</v>
+        <v>0.43347067512657983</v>
       </c>
       <c r="AB11" s="2">
         <f t="shared" si="1"/>
@@ -2224,27 +2224,27 @@
         <v>9.2606978506796338</v>
       </c>
       <c r="T12" s="4">
-        <v>0.46079999999999999</v>
+        <v>0.40589999999999998</v>
       </c>
       <c r="U12" s="4">
         <f t="shared" si="7"/>
-        <v>2.3040000000000001E-2</v>
+        <v>2.0295000000000001E-2</v>
       </c>
       <c r="V12" s="2">
         <f>L12/(L2*T12*B27*B25)</f>
-        <v>1.0734376676078054E-25</v>
+        <v>1.2871196389114671E-25</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="14"/>
-        <v>0.10734376676078054</v>
+        <v>0.1287119638911467</v>
       </c>
       <c r="X12" s="2">
         <f>SQRT(POWER(M12/(L2*T12*B27*B25),2)+POWER(L12*M2/(POWER(L2,2)*T12*B27*B25),2)+POWER(L12*C27/(L2*T12*POWER(B27,2)*B25),2)+POWER(L12*C25/(L2*T12*B27*POWER(B25,2)),2)+POWER(L12*U12/(L2*POWER(T12,2)*B27*B25),2))</f>
-        <v>2.3772614603616846E-26</v>
+        <v>2.8504868096140109E-26</v>
       </c>
       <c r="Y12" s="11">
         <f t="shared" si="8"/>
-        <v>2.3772614603616845E-2</v>
+        <v>2.8504868096140109E-2</v>
       </c>
       <c r="Z12" s="11">
         <f t="shared" si="9"/>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="AA12" s="13">
         <f t="shared" si="10"/>
-        <v>1.8263993819538786</v>
+        <v>3.5220628453629339</v>
       </c>
       <c r="AB12" s="2">
         <f t="shared" si="1"/>
@@ -2328,27 +2328,27 @@
         <v>9.0111787685075715</v>
       </c>
       <c r="T13" s="4">
-        <v>0.48780000000000001</v>
+        <v>0.42120000000000002</v>
       </c>
       <c r="U13" s="4">
         <f t="shared" si="7"/>
-        <v>2.4390000000000002E-2</v>
+        <v>2.1060000000000002E-2</v>
       </c>
       <c r="V13" s="2">
         <f>L13/(L2*T13*B27*B25)</f>
-        <v>8.1639675082086461E-26</v>
+        <v>9.9862714708137599E-26</v>
       </c>
       <c r="W13" s="11">
         <f t="shared" si="14"/>
-        <v>8.1639675082086458E-2</v>
+        <v>9.9862714708137595E-2</v>
       </c>
       <c r="X13" s="2">
         <f>SQRT(POWER(M13/(L2*T13*B27*B25),2)+POWER(L13*M2/(POWER(L2,2)*T13*B27*B25),2)+POWER(L13*C27/(L2*T13*POWER(B27,2)*B25),2)+POWER(L13*C25/(L2*T13*B27*POWER(B25,2)),2)+POWER(L13*U13/(L2*POWER(T13,2)*B27*B25),2))</f>
-        <v>1.5344371520184826E-26</v>
+        <v>1.8769435252592228E-26</v>
       </c>
       <c r="Y13" s="11">
         <f t="shared" si="8"/>
-        <v>1.5344371520184827E-2</v>
+        <v>1.8769435252592226E-2</v>
       </c>
       <c r="Z13" s="11">
         <f t="shared" si="9"/>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="AA13" s="13">
         <f t="shared" si="10"/>
-        <v>1.246757373266189</v>
+        <v>3.5483893779605085</v>
       </c>
       <c r="AB13" s="2">
         <f t="shared" si="1"/>
@@ -2440,19 +2440,19 @@
       </c>
       <c r="V14" s="2">
         <f>L14/(L2*T14*B27*B25)</f>
-        <v>7.8447598655060789E-26</v>
+        <v>8.285683136635227E-26</v>
       </c>
       <c r="W14" s="11">
         <f t="shared" si="14"/>
-        <v>7.8447598655060791E-2</v>
+        <v>8.2856831366352274E-2</v>
       </c>
       <c r="X14" s="2">
         <f>SQRT(POWER(M14/(L2*T14*B27*B25),2)+POWER(L14*M2/(POWER(L2,2)*T14*B27*B25),2)+POWER(L14*C27/(L2*T14*POWER(B27,2)*B25),2)+POWER(L14*C25/(L2*T14*B27*POWER(B25,2)),2))+POWER(L14*U14/(L2*POWER(T14,2)*B27*B25),2)</f>
-        <v>1.3939496969267884E-26</v>
+        <v>1.4722981576439854E-26</v>
       </c>
       <c r="Y14" s="11">
         <f t="shared" si="8"/>
-        <v>1.3939496969267884E-2</v>
+        <v>1.4722981576439854E-2</v>
       </c>
       <c r="Z14" s="11">
         <f t="shared" si="9"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="AA14" s="13">
         <f t="shared" si="10"/>
-        <v>3.8229045542098246</v>
+        <v>4.6253259425271134</v>
       </c>
       <c r="AB14" s="2">
         <f t="shared" si="1"/>
@@ -2544,19 +2544,19 @@
       </c>
       <c r="V15" s="2">
         <f>L15/(L2*T15*B27*B25)</f>
-        <v>6.1051228058312059E-26</v>
+        <v>6.4482678815687928E-26</v>
       </c>
       <c r="W15" s="11">
         <f t="shared" si="14"/>
-        <v>6.1051228058312056E-2</v>
+        <v>6.4482678815687922E-2</v>
       </c>
       <c r="X15" s="2">
         <f>SQRT(POWER(M15/(L2*T15*B27*B25),2)+POWER(L15*M2/(POWER(L2,2)*T15*B27*B25),2)+POWER(L15*C27/(L2*T15*POWER(B27,2)*B25),2)+POWER(L15*C25/(L2*T15*B27*POWER(B25,2)),2)+POWER(L15*U15/(L2*POWER(T15,2)*B27*B25),2))</f>
-        <v>1.1073256759218936E-26</v>
+        <v>1.1695641214069653E-26</v>
       </c>
       <c r="Y15" s="11">
         <f t="shared" si="8"/>
-        <v>1.1073256759218936E-2</v>
+        <v>1.1695641214069652E-2</v>
       </c>
       <c r="Z15" s="11">
         <f t="shared" si="9"/>
@@ -2564,7 +2564,7 @@
       </c>
       <c r="AA15" s="13">
         <f t="shared" si="10"/>
-        <v>4.0522934694670854</v>
+        <v>4.8369337412351046</v>
       </c>
       <c r="AB15" s="2">
         <f t="shared" si="1"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="K20" s="4">
         <f>SUM(AA3:AA15)</f>
-        <v>26.738956960082977</v>
+        <v>40.353216773559012</v>
       </c>
       <c r="L20" s="4">
         <f>SUM(S2:S15)</f>
@@ -2693,7 +2693,7 @@
       </c>
       <c r="K22">
         <f>K20/K21</f>
-        <v>2.0568428430833059</v>
+        <v>3.1040935979660778</v>
       </c>
       <c r="L22">
         <f>L20/L21</f>
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B26" s="2">
         <f>L2</f>
-        <v>7783.1935267008639</v>
+        <v>7369.0102791602403</v>
       </c>
       <c r="C26" s="2">
         <f>M2</f>
-        <v>779.37144102001753</v>
+        <v>737.89712930276619</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2868,7 +2868,6 @@
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>